<commit_message>
Collected timings for CUG of RA and STREAM.
git-svn-id: http://svn.code.sf.net/p/chapel/code/trunk@15514 3a8e244f-b0f2-452b-bcba-4c88e055c3ca
</commit_message>
<xml_diff>
--- a/doc/timings/CUG09_STREAM_RA.xlsx
+++ b/doc/timings/CUG09_STREAM_RA.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -200,7 +199,7 @@
                   <c:v>1.4013000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3481199999999998E-4</c:v>
+                  <c:v>3.3522100000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6.2692299999999996E-5</c:v>
@@ -209,19 +208,19 @@
                   <c:v>7.4051100000000007E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.01394E-4</c:v>
+                  <c:v>1.25556E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0948399999999999E-4</c:v>
+                  <c:v>2.3286800000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8049999999999998E-4</c:v>
+                  <c:v>4.3358999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>8.52771E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.65536E-3</c:v>
+                  <c:v>1.6780199999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.2410099999999999E-3</c:v>
@@ -304,28 +303,28 @@
                   <c:v>4.86551E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.2656499999999998E-5</c:v>
+                  <c:v>7.7851999999999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.7479799999999997E-5</c:v>
+                  <c:v>6.9599599999999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8.9864900000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3216899999999999E-4</c:v>
+                  <c:v>1.5408800000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6729100000000001E-4</c:v>
+                  <c:v>2.8940699999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.8079200000000001E-4</c:v>
+                  <c:v>5.4991600000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.8148000000000007E-4</c:v>
+                  <c:v>1.0692399999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0745799999999999E-3</c:v>
+                  <c:v>2.0863000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>4.1475799999999997E-3</c:v>
@@ -408,7 +407,7 @@
                   <c:v>2.4566399999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3096300000000001E-5</c:v>
+                  <c:v>6.3382700000000006E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7.0180900000000004E-5</c:v>
@@ -417,16 +416,16 @@
                   <c:v>9.4627400000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4128799999999999E-4</c:v>
+                  <c:v>1.62017E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.8118799999999998E-4</c:v>
+                  <c:v>3.0818000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.4430899999999998E-4</c:v>
+                  <c:v>5.8352999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.5976499999999998E-4</c:v>
+                  <c:v>1.1386499999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2.2137200000000002E-3</c:v>
@@ -512,7 +511,7 @@
                   <c:v>1.5756E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.67668E-5</c:v>
+                  <c:v>5.7362699999999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6.9709399999999994E-5</c:v>
@@ -521,13 +520,13 @@
                   <c:v>9.5049600000000006E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.50617E-4</c:v>
+                  <c:v>1.6543499999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.9715699999999999E-4</c:v>
+                  <c:v>3.1070499999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.6183299999999997E-4</c:v>
+                  <c:v>5.9864900000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.1572100000000001E-3</c:v>
@@ -625,19 +624,19 @@
                   <c:v>9.76926E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5508500000000001E-4</c:v>
+                  <c:v>1.6897799999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0682600000000001E-4</c:v>
+                  <c:v>3.1694900000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.9025500000000003E-4</c:v>
+                  <c:v>6.1062300000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.1819199999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.07909E-3</c:v>
+                  <c:v>2.30701E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>4.4786299999999999E-3</c:v>
@@ -653,11 +652,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="12629888"/>
-        <c:axId val="12637312"/>
+        <c:axId val="73100288"/>
+        <c:axId val="73111040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="12629888"/>
+        <c:axId val="73100288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,17 +687,17 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="12637312"/>
+        <c:crossAx val="73111040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12637312"/>
+        <c:axId val="73111040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.8000000000000016E-2"/>
+          <c:max val="1.8000000000000023E-2"/>
           <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
@@ -723,10 +722,10 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="12629888"/>
+        <c:crossAx val="73100288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="3.0000000000000022E-3"/>
+        <c:majorUnit val="3.0000000000000035E-3"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -737,7 +736,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -837,7 +836,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.23892956540355381</c:v>
+                  <c:v>0.23922143723685149</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.2369335616927135E-2</c:v>
@@ -846,19 +845,19 @@
                   <c:v>1.3211143224149005E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.0446371226718045E-3</c:v>
+                  <c:v>1.1199957182616141E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.343288375080281E-3</c:v>
+                  <c:v>1.0386248483550988E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.4854242489117247E-3</c:v>
+                  <c:v>9.6693695140226913E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>9.508703971312352E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.2289302790266176E-3</c:v>
+                  <c:v>9.3552638621280226E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>9.0346073735103113E-3</c:v>
@@ -941,28 +940,28 @@
                   <c:v>0.34721401555698278</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1849354171126807E-2</c:v>
+                  <c:v>5.5556982801684147E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4077570827089129E-2</c:v>
+                  <c:v>2.4833939912937985E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.6032416327695712E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1789855848141011E-2</c:v>
+                  <c:v>1.3745093841432954E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1921563904945408E-2</c:v>
+                  <c:v>1.2907969385570541E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0722008135302932E-2</c:v>
+                  <c:v>1.2263523157068437E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.09438557054164E-2</c:v>
+                  <c:v>1.192241133233426E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.1566157318204524E-2</c:v>
+                  <c:v>1.1631498430029259E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1.1561752925854563E-2</c:v>
@@ -1045,7 +1044,7 @@
                   <c:v>0.1753114964675658</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5026974951830438E-2</c:v>
+                  <c:v>4.5231356597445233E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.5041354456576036E-2</c:v>
@@ -1054,16 +1053,16 @@
                   <c:v>1.6882073788624847E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2603296938557053E-2</c:v>
+                  <c:v>1.4452383501034753E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2541390137729249E-2</c:v>
+                  <c:v>1.374527224719903E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2138483015771069E-2</c:v>
+                  <c:v>1.3013139584671376E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.356617515878113E-3</c:v>
+                  <c:v>1.269635784628559E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.23418878898166E-2</c:v>
@@ -1149,7 +1148,7 @@
                   <c:v>0.11243845001070434</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0510097766359804E-2</c:v>
+                  <c:v>4.0935345750374649E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.4873117819167911E-2</c:v>
@@ -1158,13 +1157,13 @@
                   <c:v>1.6957396703061442E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3435470634410904E-2</c:v>
+                  <c:v>1.4757278955255831E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3253630557339613E-2</c:v>
+                  <c:v>1.3857890887033467E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2529280846356954E-2</c:v>
+                  <c:v>1.3350304181831156E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.2903308534931849E-2</c:v>
@@ -1262,19 +1261,19 @@
                   <c:v>1.7428923142795975E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3834029115821024E-2</c:v>
+                  <c:v>1.5073324769856561E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3684881895382858E-2</c:v>
+                  <c:v>1.4136382287875544E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3163111931777636E-2</c:v>
+                  <c:v>1.3617333012202954E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.3178833939912937E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.159130138086063E-2</c:v>
+                  <c:v>1.2861996449725254E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1.2484584626775137E-2</c:v>
@@ -1290,11 +1289,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="110461696"/>
-        <c:axId val="110621056"/>
+        <c:axId val="73433856"/>
+        <c:axId val="73435776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110461696"/>
+        <c:axId val="73433856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1320,14 +1319,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110621056"/>
+        <c:crossAx val="73435776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110621056"/>
+        <c:axId val="73435776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1363,7 +1362,7 @@
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110461696"/>
+        <c:crossAx val="73433856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -1377,7 +1376,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1475,19 +1474,19 @@
                   <c:v>0.51666057334866444</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35371711003695067</c:v>
+                  <c:v>0.43800723383828805</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3653967447727704</c:v>
+                  <c:v>0.40618476428627248</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.33184744750443745</c:v>
+                  <c:v>0.37814910581721162</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.37186580769488387</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.36092443541455033</c:v>
+                  <c:v>0.36586508138068075</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.3533248672261356</c:v>
@@ -1562,25 +1561,25 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.94162415298228386</c:v>
+                  <c:v>0.97120418848167545</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.62699474765290975</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.46107695442012075</c:v>
+                  <c:v>0.53754228111499358</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4662277849719243</c:v>
+                  <c:v>0.50480406959220359</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.41931563201196714</c:v>
+                  <c:v>0.47960110628607155</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.42799163308364691</c:v>
+                  <c:v>0.46626092610991415</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45232856612598937</c:v>
+                  <c:v>0.4548839222920551</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.45215631942196272</c:v>
@@ -1661,16 +1660,16 @@
                   <c:v>0.66022309916386657</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.49288895834961322</c:v>
+                  <c:v>0.56520292144364193</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.49046791100592774</c:v>
+                  <c:v>0.53754925819667565</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.47471104416213622</c:v>
+                  <c:v>0.50891705924379593</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.28770214349903439</c:v>
+                  <c:v>0.49652837858203375</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.48266578941492994</c:v>
@@ -1754,13 +1753,13 @@
                   <c:v>0.66316882305004532</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.52543355585572515</c:v>
+                  <c:v>0.57712675403833491</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51832216535125419</c:v>
+                  <c:v>0.54195354100849535</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.48999434158675581</c:v>
+                  <c:v>0.52210287148773715</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.50462179333325896</c:v>
@@ -1847,19 +1846,19 @@
                   <c:v>0.68160924993581085</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54102035633351575</c:v>
+                  <c:v>0.58948665423815849</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.53518751604728787</c:v>
+                  <c:v>0.55284476551423889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.51478216853280356</c:v>
+                  <c:v>0.53254581849540639</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.51539702385603769</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45331189857555904</c:v>
+                  <c:v>0.50300616285624977</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.4882463645915896</c:v>
@@ -1875,11 +1874,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="98260864"/>
-        <c:axId val="98275712"/>
+        <c:axId val="73463680"/>
+        <c:axId val="72896512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98260864"/>
+        <c:axId val="73463680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1906,14 +1905,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98275712"/>
+        <c:crossAx val="72896512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98275712"/>
+        <c:axId val="72896512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1950,7 +1949,7 @@
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98260864"/>
+        <c:crossAx val="73463680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -1964,7 +1963,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2070,16 +2069,16 @@
                   <c:v>7.9857500000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.834199999999999</c:v>
+                  <c:v>15.862299999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.331800000000001</c:v>
+                  <c:v>30.935600000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>63.344999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.244</c:v>
+                  <c:v>125.366</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>253.244</c:v>
@@ -2178,10 +2177,10 @@
                   <c:v>92.366299999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>184.50299999999999</c:v>
+                  <c:v>185.36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>365.94200000000001</c:v>
+                  <c:v>368.91800000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>728.92899999999997</c:v>
@@ -2271,7 +2270,7 @@
                   <c:v>24.011700000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44.744</c:v>
+                  <c:v>47.935099999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>95.772400000000005</c:v>
@@ -2283,7 +2282,7 @@
                   <c:v>381.137</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>746.83799999999997</c:v>
+                  <c:v>763.86599999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1510.7</c:v>
@@ -2361,25 +2360,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>5.9626000000000001</c:v>
+                  <c:v>6.1149899999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.738300000000001</c:v>
+                  <c:v>12.194900000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.6144</c:v>
+                  <c:v>24.378599999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46.509599999999999</c:v>
+                  <c:v>48.820500000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>93.003500000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>170.16800000000001</c:v>
+                  <c:v>185.57499999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>365.15899999999999</c:v>
+                  <c:v>369.42399999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>747.11699999999996</c:v>
@@ -2460,16 +2459,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>5.4567300000000003</c:v>
+                  <c:v>5.5192300000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.7302</c:v>
+                  <c:v>11.0251</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.359300000000001</c:v>
+                  <c:v>22.000900000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.6813</c:v>
+                  <c:v>43.991900000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>85.230599999999995</c:v>
@@ -2497,11 +2496,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="115443200"/>
-        <c:axId val="115445120"/>
+        <c:axId val="73473024"/>
+        <c:axId val="73479296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115443200"/>
+        <c:axId val="73473024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2528,14 +2527,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115445120"/>
+        <c:crossAx val="73479296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115445120"/>
+        <c:axId val="73479296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6000"/>
@@ -2562,7 +2561,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115443200"/>
+        <c:crossAx val="73473024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2575,7 +2574,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2681,16 +2680,16 @@
                   <c:v>0.65207149004551412</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.64646591664393949</c:v>
+                  <c:v>0.6476131607268546</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.59876750874110174</c:v>
+                  <c:v>0.63150683365532378</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.64654961238664321</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.63917009751166431</c:v>
+                  <c:v>0.63979271218299727</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.64620258125835928</c:v>
@@ -2789,10 +2788,10 @@
                   <c:v>0.94276415601213048</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.94159241561427764</c:v>
+                  <c:v>0.94596602851044442</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.93377400842999847</c:v>
+                  <c:v>0.94136786606068223</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.93000387245911964</c:v>
@@ -2882,7 +2881,7 @@
                   <c:v>0.98033027564886654</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.91338592964331722</c:v>
+                  <c:v>0.97852775514136814</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.97752953030765732</c:v>
@@ -2894,7 +2893,7 @@
                   <c:v>0.97254708191731021</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.95285306538719683</c:v>
+                  <c:v>0.97457823469756022</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.96371309834290586</c:v>
@@ -2972,25 +2971,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.97374484964978425</c:v>
+                  <c:v>0.99863147253881435</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95848364544360376</c:v>
+                  <c:v>0.99576703677876721</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.96410963244095971</c:v>
+                  <c:v>0.99530977223326356</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.94942817435497107</c:v>
+                  <c:v>0.99660195284622677</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.94926792762808709</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.86843519173265704</c:v>
+                  <c:v>0.94706325928369495</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.93177602774289314</c:v>
+                  <c:v>0.9426590259938562</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.95320902746363512</c:v>
@@ -3071,16 +3070,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.89113184406625767</c:v>
+                  <c:v>0.90133864195696156</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.87616786181465434</c:v>
+                  <c:v>0.90024773939840308</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.87204023274765363</c:v>
+                  <c:v>0.89823495885435634</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.87127880562500704</c:v>
+                  <c:v>0.89803286425612039</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.86993150830343413</c:v>
@@ -3108,11 +3107,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="98326784"/>
-        <c:axId val="101177984"/>
+        <c:axId val="73523584"/>
+        <c:axId val="73525504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98326784"/>
+        <c:axId val="73523584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3139,14 +3138,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101177984"/>
+        <c:crossAx val="73525504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101177984"/>
+        <c:axId val="73525504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3188,7 +3187,7 @@
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98326784"/>
+        <c:crossAx val="73523584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -3202,7 +3201,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3651,7 +3650,7 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3773,16 +3772,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>3.3481199999999998E-4</v>
+        <v>3.3522100000000002E-4</v>
       </c>
       <c r="C4" s="1">
-        <v>7.2656499999999998E-5</v>
+        <v>7.7851999999999999E-5</v>
       </c>
       <c r="D4" s="1">
-        <v>6.3096300000000001E-5</v>
+        <v>6.3382700000000006E-5</v>
       </c>
       <c r="E4" s="1">
-        <v>5.67668E-5</v>
+        <v>5.7362699999999999E-5</v>
       </c>
       <c r="F4" s="1">
         <v>6.1305100000000004E-5</v>
@@ -3793,19 +3792,19 @@
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H14" si="0">B4/G4</f>
-        <v>0.23892956540355381</v>
+        <v>0.23922143723685149</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I14" si="1">C4/G4</f>
-        <v>5.1849354171126807E-2</v>
+        <v>5.5556982801684147E-2</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J14" si="2">D4/G4</f>
-        <v>4.5026974951830438E-2</v>
+        <v>4.5231356597445233E-2</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K14" si="3">E4/G4</f>
-        <v>4.0510097766359804E-2</v>
+        <v>4.0935345750374649E-2</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L14" si="4">F4/G4</f>
@@ -3828,7 +3827,7 @@
         <v>6.2692299999999996E-5</v>
       </c>
       <c r="C5" s="1">
-        <v>6.7479799999999997E-5</v>
+        <v>6.9599599999999997E-5</v>
       </c>
       <c r="D5" s="1">
         <v>7.0180900000000004E-5</v>
@@ -3840,7 +3839,7 @@
         <v>7.1663199999999995E-5</v>
       </c>
       <c r="G5" s="1">
-        <f>G4*2</f>
+        <f t="shared" ref="G5:G14" si="5">G4*2</f>
         <v>2.8026000000000001E-3</v>
       </c>
       <c r="H5">
@@ -3849,7 +3848,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>2.4077570827089129E-2</v>
+        <v>2.4833939912937985E-2</v>
       </c>
       <c r="J5">
         <f t="shared" si="2"/>
@@ -3873,7 +3872,7 @@
       </c>
       <c r="O5" s="1">
         <f>C5/M5</f>
-        <v>0.94162415298228386</v>
+        <v>0.97120418848167545</v>
       </c>
       <c r="P5" s="1">
         <f>D5/M5</f>
@@ -3910,7 +3909,7 @@
         <v>9.76926E-5</v>
       </c>
       <c r="G6" s="1">
-        <f>G5*2</f>
+        <f t="shared" si="5"/>
         <v>5.6052000000000003E-3</v>
       </c>
       <c r="H6">
@@ -3934,27 +3933,27 @@
         <v>1.7428923142795975E-2</v>
       </c>
       <c r="M6" s="1">
-        <f>M5*2</f>
+        <f t="shared" ref="M6:M14" si="6">M5*2</f>
         <v>1.4332639999999999E-4</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" ref="N6:N14" si="5">B6/M6</f>
+        <f t="shared" ref="N6:N14" si="7">B6/M6</f>
         <v>0.51666057334866444</v>
       </c>
       <c r="O6" s="1">
-        <f t="shared" ref="O6:O14" si="6">C6/M6</f>
+        <f t="shared" ref="O6:O14" si="8">C6/M6</f>
         <v>0.62699474765290975</v>
       </c>
       <c r="P6" s="1">
-        <f t="shared" ref="P6:P14" si="7">D6/M6</f>
+        <f t="shared" ref="P6:P14" si="9">D6/M6</f>
         <v>0.66022309916386657</v>
       </c>
       <c r="Q6" s="1">
-        <f t="shared" ref="Q6:Q14" si="8">E6/M6</f>
+        <f t="shared" ref="Q6:Q14" si="10">E6/M6</f>
         <v>0.66316882305004532</v>
       </c>
       <c r="R6" s="1">
-        <f t="shared" ref="R6:R14" si="9">F6/M6</f>
+        <f t="shared" ref="R6:R14" si="11">F6/M6</f>
         <v>0.68160924993581085</v>
       </c>
       <c r="S6" s="1"/>
@@ -3965,67 +3964,67 @@
         <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>1.01394E-4</v>
+        <v>1.25556E-4</v>
       </c>
       <c r="C7" s="1">
-        <v>1.3216899999999999E-4</v>
+        <v>1.5408800000000001E-4</v>
       </c>
       <c r="D7" s="1">
-        <v>1.4128799999999999E-4</v>
+        <v>1.62017E-4</v>
       </c>
       <c r="E7" s="1">
-        <v>1.50617E-4</v>
+        <v>1.6543499999999999E-4</v>
       </c>
       <c r="F7" s="1">
-        <v>1.5508500000000001E-4</v>
+        <v>1.6897799999999999E-4</v>
       </c>
       <c r="G7" s="1">
-        <f>G6*2</f>
+        <f t="shared" si="5"/>
         <v>1.1210400000000001E-2</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>9.0446371226718045E-3</v>
+        <v>1.1199957182616141E-2</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>1.1789855848141011E-2</v>
+        <v>1.3745093841432954E-2</v>
       </c>
       <c r="J7">
         <f t="shared" si="2"/>
-        <v>1.2603296938557053E-2</v>
+        <v>1.4452383501034753E-2</v>
       </c>
       <c r="K7">
         <f t="shared" si="3"/>
-        <v>1.3435470634410904E-2</v>
+        <v>1.4757278955255831E-2</v>
       </c>
       <c r="L7">
         <f t="shared" si="4"/>
-        <v>1.3834029115821024E-2</v>
+        <v>1.5073324769856561E-2</v>
       </c>
       <c r="M7" s="1">
-        <f>M6*2</f>
+        <f t="shared" si="6"/>
         <v>2.8665279999999998E-4</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="5"/>
-        <v>0.35371711003695067</v>
+        <f t="shared" si="7"/>
+        <v>0.43800723383828805</v>
       </c>
       <c r="O7" s="1">
-        <f t="shared" si="6"/>
-        <v>0.46107695442012075</v>
+        <f t="shared" si="8"/>
+        <v>0.53754228111499358</v>
       </c>
       <c r="P7" s="1">
-        <f t="shared" si="7"/>
-        <v>0.49288895834961322</v>
+        <f t="shared" si="9"/>
+        <v>0.56520292144364193</v>
       </c>
       <c r="Q7" s="1">
-        <f t="shared" si="8"/>
-        <v>0.52543355585572515</v>
+        <f t="shared" si="10"/>
+        <v>0.57712675403833491</v>
       </c>
       <c r="R7" s="1">
-        <f t="shared" si="9"/>
-        <v>0.54102035633351575</v>
+        <f t="shared" si="11"/>
+        <v>0.58948665423815849</v>
       </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -4035,67 +4034,67 @@
         <v>16</v>
       </c>
       <c r="B8" s="1">
-        <v>2.0948399999999999E-4</v>
+        <v>2.3286800000000001E-4</v>
       </c>
       <c r="C8" s="1">
-        <v>2.6729100000000001E-4</v>
+        <v>2.8940699999999999E-4</v>
       </c>
       <c r="D8" s="1">
-        <v>2.8118799999999998E-4</v>
+        <v>3.0818000000000002E-4</v>
       </c>
       <c r="E8" s="1">
-        <v>2.9715699999999999E-4</v>
+        <v>3.1070499999999999E-4</v>
       </c>
       <c r="F8" s="1">
-        <v>3.0682600000000001E-4</v>
+        <v>3.1694900000000002E-4</v>
       </c>
       <c r="G8" s="1">
-        <f>G7*2</f>
+        <f t="shared" si="5"/>
         <v>2.2420800000000001E-2</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>9.343288375080281E-3</v>
+        <v>1.0386248483550988E-2</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>1.1921563904945408E-2</v>
+        <v>1.2907969385570541E-2</v>
       </c>
       <c r="J8">
         <f t="shared" si="2"/>
-        <v>1.2541390137729249E-2</v>
+        <v>1.374527224719903E-2</v>
       </c>
       <c r="K8">
         <f t="shared" si="3"/>
-        <v>1.3253630557339613E-2</v>
+        <v>1.3857890887033467E-2</v>
       </c>
       <c r="L8">
         <f t="shared" si="4"/>
-        <v>1.3684881895382858E-2</v>
+        <v>1.4136382287875544E-2</v>
       </c>
       <c r="M8" s="1">
-        <f>M7*2</f>
+        <f t="shared" si="6"/>
         <v>5.7330559999999996E-4</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="5"/>
-        <v>0.3653967447727704</v>
+        <f t="shared" si="7"/>
+        <v>0.40618476428627248</v>
       </c>
       <c r="O8" s="1">
-        <f t="shared" si="6"/>
-        <v>0.4662277849719243</v>
+        <f t="shared" si="8"/>
+        <v>0.50480406959220359</v>
       </c>
       <c r="P8" s="1">
-        <f t="shared" si="7"/>
-        <v>0.49046791100592774</v>
+        <f t="shared" si="9"/>
+        <v>0.53754925819667565</v>
       </c>
       <c r="Q8" s="1">
-        <f t="shared" si="8"/>
-        <v>0.51832216535125419</v>
+        <f t="shared" si="10"/>
+        <v>0.54195354100849535</v>
       </c>
       <c r="R8" s="1">
-        <f t="shared" si="9"/>
-        <v>0.53518751604728787</v>
+        <f t="shared" si="11"/>
+        <v>0.55284476551423889</v>
       </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
@@ -4105,67 +4104,67 @@
         <v>32</v>
       </c>
       <c r="B9" s="1">
-        <v>3.8049999999999998E-4</v>
+        <v>4.3358999999999997E-4</v>
       </c>
       <c r="C9" s="1">
-        <v>4.8079200000000001E-4</v>
+        <v>5.4991600000000001E-4</v>
       </c>
       <c r="D9" s="1">
-        <v>5.4430899999999998E-4</v>
+        <v>5.8352999999999996E-4</v>
       </c>
       <c r="E9" s="1">
-        <v>5.6183299999999997E-4</v>
+        <v>5.9864900000000003E-4</v>
       </c>
       <c r="F9" s="1">
-        <v>5.9025500000000003E-4</v>
+        <v>6.1062300000000003E-4</v>
       </c>
       <c r="G9" s="1">
-        <f>G8*2</f>
+        <f t="shared" si="5"/>
         <v>4.4841600000000002E-2</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>8.4854242489117247E-3</v>
+        <v>9.6693695140226913E-3</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
-        <v>1.0722008135302932E-2</v>
+        <v>1.2263523157068437E-2</v>
       </c>
       <c r="J9">
         <f t="shared" si="2"/>
-        <v>1.2138483015771069E-2</v>
+        <v>1.3013139584671376E-2</v>
       </c>
       <c r="K9">
         <f t="shared" si="3"/>
-        <v>1.2529280846356954E-2</v>
+        <v>1.3350304181831156E-2</v>
       </c>
       <c r="L9">
         <f t="shared" si="4"/>
-        <v>1.3163111931777636E-2</v>
+        <v>1.3617333012202954E-2</v>
       </c>
       <c r="M9" s="1">
-        <f>M8*2</f>
+        <f t="shared" si="6"/>
         <v>1.1466111999999999E-3</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="5"/>
-        <v>0.33184744750443745</v>
+        <f t="shared" si="7"/>
+        <v>0.37814910581721162</v>
       </c>
       <c r="O9" s="1">
-        <f t="shared" si="6"/>
-        <v>0.41931563201196714</v>
+        <f t="shared" si="8"/>
+        <v>0.47960110628607155</v>
       </c>
       <c r="P9" s="1">
-        <f t="shared" si="7"/>
-        <v>0.47471104416213622</v>
+        <f t="shared" si="9"/>
+        <v>0.50891705924379593</v>
       </c>
       <c r="Q9" s="1">
-        <f t="shared" si="8"/>
-        <v>0.48999434158675581</v>
+        <f t="shared" si="10"/>
+        <v>0.52210287148773715</v>
       </c>
       <c r="R9" s="1">
-        <f t="shared" si="9"/>
-        <v>0.51478216853280356</v>
+        <f t="shared" si="11"/>
+        <v>0.53254581849540639</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -4178,10 +4177,10 @@
         <v>8.52771E-4</v>
       </c>
       <c r="C10" s="1">
-        <v>9.8148000000000007E-4</v>
+        <v>1.0692399999999999E-3</v>
       </c>
       <c r="D10" s="1">
-        <v>6.5976499999999998E-4</v>
+        <v>1.1386499999999999E-3</v>
       </c>
       <c r="E10" s="1">
         <v>1.1572100000000001E-3</v>
@@ -4190,7 +4189,7 @@
         <v>1.1819199999999999E-3</v>
       </c>
       <c r="G10" s="1">
-        <f>G9*2</f>
+        <f t="shared" si="5"/>
         <v>8.9683200000000005E-2</v>
       </c>
       <c r="H10">
@@ -4199,11 +4198,11 @@
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
-        <v>1.09438557054164E-2</v>
+        <v>1.192241133233426E-2</v>
       </c>
       <c r="J10">
         <f t="shared" si="2"/>
-        <v>7.356617515878113E-3</v>
+        <v>1.269635784628559E-2</v>
       </c>
       <c r="K10">
         <f t="shared" si="3"/>
@@ -4214,27 +4213,27 @@
         <v>1.3178833939912937E-2</v>
       </c>
       <c r="M10" s="1">
-        <f>M9*2</f>
+        <f t="shared" si="6"/>
         <v>2.2932223999999998E-3</v>
       </c>
       <c r="N10" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.37186580769488387</v>
       </c>
       <c r="O10" s="1">
-        <f t="shared" si="6"/>
-        <v>0.42799163308364691</v>
+        <f t="shared" si="8"/>
+        <v>0.46626092610991415</v>
       </c>
       <c r="P10" s="1">
-        <f t="shared" si="7"/>
-        <v>0.28770214349903439</v>
+        <f t="shared" si="9"/>
+        <v>0.49652837858203375</v>
       </c>
       <c r="Q10" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.50462179333325896</v>
       </c>
       <c r="R10" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.51539702385603769</v>
       </c>
       <c r="S10" s="1"/>
@@ -4245,10 +4244,10 @@
         <v>128</v>
       </c>
       <c r="B11" s="1">
-        <v>1.65536E-3</v>
+        <v>1.6780199999999999E-3</v>
       </c>
       <c r="C11" s="1">
-        <v>2.0745799999999999E-3</v>
+        <v>2.0863000000000001E-3</v>
       </c>
       <c r="D11" s="1">
         <v>2.2137200000000002E-3</v>
@@ -4257,19 +4256,19 @@
         <v>2.26151E-3</v>
       </c>
       <c r="F11" s="1">
-        <v>2.07909E-3</v>
+        <v>2.30701E-3</v>
       </c>
       <c r="G11" s="1">
-        <f>G10*2</f>
+        <f t="shared" si="5"/>
         <v>0.17936640000000001</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>9.2289302790266176E-3</v>
+        <v>9.3552638621280226E-3</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
-        <v>1.1566157318204524E-2</v>
+        <v>1.1631498430029259E-2</v>
       </c>
       <c r="J11">
         <f t="shared" si="2"/>
@@ -4281,31 +4280,31 @@
       </c>
       <c r="L11">
         <f t="shared" si="4"/>
-        <v>1.159130138086063E-2</v>
+        <v>1.2861996449725254E-2</v>
       </c>
       <c r="M11" s="1">
-        <f>M10*2</f>
+        <f t="shared" si="6"/>
         <v>4.5864447999999997E-3</v>
       </c>
       <c r="N11" s="1">
-        <f t="shared" si="5"/>
-        <v>0.36092443541455033</v>
+        <f t="shared" si="7"/>
+        <v>0.36586508138068075</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" si="6"/>
-        <v>0.45232856612598937</v>
+        <f t="shared" si="8"/>
+        <v>0.4548839222920551</v>
       </c>
       <c r="P11" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.48266578941492994</v>
       </c>
       <c r="Q11" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.49308562483952717</v>
       </c>
       <c r="R11" s="1">
-        <f t="shared" si="9"/>
-        <v>0.45331189857555904</v>
+        <f t="shared" si="11"/>
+        <v>0.50300616285624977</v>
       </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
@@ -4330,7 +4329,7 @@
         <v>4.4786299999999999E-3</v>
       </c>
       <c r="G12" s="1">
-        <f>G11*2</f>
+        <f t="shared" si="5"/>
         <v>0.35873280000000002</v>
       </c>
       <c r="H12">
@@ -4354,27 +4353,27 @@
         <v>1.2484584626775137E-2</v>
       </c>
       <c r="M12" s="1">
-        <f>M11*2</f>
+        <f t="shared" si="6"/>
         <v>9.1728895999999994E-3</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.3533248672261356</v>
       </c>
       <c r="O12" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.45215631942196272</v>
       </c>
       <c r="P12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.45390168001149828</v>
       </c>
       <c r="Q12" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.48658385684702893</v>
       </c>
       <c r="R12" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.4882463645915896</v>
       </c>
       <c r="S12" s="1"/>
@@ -4400,7 +4399,7 @@
         <v>9.0095899999999996E-3</v>
       </c>
       <c r="G13" s="1">
-        <f>G12*2</f>
+        <f t="shared" si="5"/>
         <v>0.71746560000000004</v>
       </c>
       <c r="H13">
@@ -4424,27 +4423,27 @@
         <v>1.2557521921608505E-2</v>
       </c>
       <c r="M13" s="1">
-        <f>M12*2</f>
+        <f t="shared" si="6"/>
         <v>1.8345779199999999E-2</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.34239919337958674</v>
       </c>
       <c r="O13" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.4373927055657576</v>
       </c>
       <c r="P13" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.40887660961274408</v>
       </c>
       <c r="Q13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.46109516024263503</v>
       </c>
       <c r="R13" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.49109879181365051</v>
       </c>
       <c r="S13" s="1"/>
@@ -4470,7 +4469,7 @@
         <v>1.5795400000000001E-2</v>
       </c>
       <c r="G14" s="1">
-        <f>G13*2</f>
+        <f t="shared" si="5"/>
         <v>1.4349312000000001</v>
       </c>
       <c r="H14">
@@ -4494,27 +4493,27 @@
         <v>1.1007775146292729E-2</v>
       </c>
       <c r="M14" s="1">
-        <f>M13*2</f>
+        <f t="shared" si="6"/>
         <v>3.6691558399999998E-2</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.32091032688325394</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.37853938632380363</v>
       </c>
       <c r="P14" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.44466358779680509</v>
       </c>
       <c r="Q14" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.43885298695843894</v>
       </c>
       <c r="R14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.43049139063005842</v>
       </c>
       <c r="S14" s="1"/>
@@ -4580,10 +4579,10 @@
         <v>6.1233700000000004</v>
       </c>
       <c r="E18">
-        <v>5.9626000000000001</v>
+        <v>6.1149899999999997</v>
       </c>
       <c r="F18">
-        <v>5.4567300000000003</v>
+        <v>5.5192300000000003</v>
       </c>
       <c r="G18">
         <f>MAX(B18:F18)</f>
@@ -4603,11 +4602,11 @@
       </c>
       <c r="K18">
         <f>E18/G18</f>
-        <v>0.97374484964978425</v>
+        <v>0.99863147253881435</v>
       </c>
       <c r="L18">
         <f>F18/G18</f>
-        <v>0.89113184406625767</v>
+        <v>0.90133864195696156</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -4624,34 +4623,34 @@
         <v>12.137499999999999</v>
       </c>
       <c r="E19">
-        <v>11.738300000000001</v>
+        <v>12.194900000000001</v>
       </c>
       <c r="F19">
-        <v>10.7302</v>
+        <v>11.0251</v>
       </c>
       <c r="G19">
-        <f>2*G18</f>
+        <f t="shared" ref="G19:G28" si="12">2*G18</f>
         <v>12.246740000000001</v>
       </c>
       <c r="H19">
-        <f t="shared" ref="H19:H28" si="10">B19/G19</f>
+        <f t="shared" ref="H19:H28" si="13">B19/G19</f>
         <v>0.65207149004551412</v>
       </c>
       <c r="I19">
-        <f t="shared" ref="I19:I28" si="11">C19/G19</f>
+        <f t="shared" ref="I19:I28" si="14">C19/G19</f>
         <v>0.9570955209304679</v>
       </c>
       <c r="J19">
-        <f t="shared" ref="J19:J28" si="12">D19/G19</f>
+        <f t="shared" ref="J19:J28" si="15">D19/G19</f>
         <v>0.99108007518735586</v>
       </c>
       <c r="K19">
-        <f t="shared" ref="K19:K28" si="13">E19/G19</f>
-        <v>0.95848364544360376</v>
+        <f t="shared" ref="K19:K28" si="16">E19/G19</f>
+        <v>0.99576703677876721</v>
       </c>
       <c r="L19">
-        <f t="shared" ref="L19:L28" si="14">F19/G19</f>
-        <v>0.87616786181465434</v>
+        <f t="shared" ref="L19:L28" si="17">F19/G19</f>
+        <v>0.90024773939840308</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -4659,7 +4658,7 @@
         <v>4</v>
       </c>
       <c r="B20">
-        <v>15.834199999999999</v>
+        <v>15.862299999999999</v>
       </c>
       <c r="C20">
         <v>23.513999999999999</v>
@@ -4668,34 +4667,34 @@
         <v>24.011700000000001</v>
       </c>
       <c r="E20">
-        <v>23.6144</v>
+        <v>24.378599999999999</v>
       </c>
       <c r="F20">
-        <v>21.359300000000001</v>
+        <v>22.000900000000001</v>
       </c>
       <c r="G20">
-        <f>2*G19</f>
+        <f t="shared" si="12"/>
         <v>24.493480000000002</v>
       </c>
       <c r="H20">
-        <f t="shared" si="10"/>
-        <v>0.64646591664393949</v>
+        <f t="shared" si="13"/>
+        <v>0.6476131607268546</v>
       </c>
       <c r="I20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.96001058240805304</v>
       </c>
       <c r="J20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.98033027564886654</v>
       </c>
       <c r="K20">
-        <f t="shared" si="13"/>
-        <v>0.96410963244095971</v>
+        <f t="shared" si="16"/>
+        <v>0.99530977223326356</v>
       </c>
       <c r="L20">
-        <f t="shared" si="14"/>
-        <v>0.87204023274765363</v>
+        <f t="shared" si="17"/>
+        <v>0.89823495885435634</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -4703,43 +4702,43 @@
         <v>8</v>
       </c>
       <c r="B21">
-        <v>29.331800000000001</v>
+        <v>30.935600000000001</v>
       </c>
       <c r="C21">
         <v>46.477699999999999</v>
       </c>
       <c r="D21">
-        <v>44.744</v>
+        <v>47.935099999999998</v>
       </c>
       <c r="E21">
-        <v>46.509599999999999</v>
+        <v>48.820500000000003</v>
       </c>
       <c r="F21">
-        <v>42.6813</v>
+        <v>43.991900000000001</v>
       </c>
       <c r="G21">
-        <f>2*G20</f>
+        <f t="shared" si="12"/>
         <v>48.986960000000003</v>
       </c>
       <c r="H21">
-        <f t="shared" si="10"/>
-        <v>0.59876750874110174</v>
+        <f t="shared" si="13"/>
+        <v>0.63150683365532378</v>
       </c>
       <c r="I21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.94877698064954419</v>
       </c>
       <c r="J21">
-        <f t="shared" si="12"/>
-        <v>0.91338592964331722</v>
+        <f t="shared" si="15"/>
+        <v>0.97852775514136814</v>
       </c>
       <c r="K21">
-        <f t="shared" si="13"/>
-        <v>0.94942817435497107</v>
+        <f t="shared" si="16"/>
+        <v>0.99660195284622677</v>
       </c>
       <c r="L21">
-        <f t="shared" si="14"/>
-        <v>0.87127880562500704</v>
+        <f t="shared" si="17"/>
+        <v>0.89803286425612039</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -4762,27 +4761,27 @@
         <v>85.230599999999995</v>
       </c>
       <c r="G22">
-        <f>2*G21</f>
+        <f t="shared" si="12"/>
         <v>97.973920000000007</v>
       </c>
       <c r="H22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.64654961238664321</v>
       </c>
       <c r="I22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.94276415601213048</v>
       </c>
       <c r="J22">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.97752953030765732</v>
       </c>
       <c r="K22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.94926792762808709</v>
       </c>
       <c r="L22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.86993150830343413</v>
       </c>
     </row>
@@ -4791,42 +4790,42 @@
         <v>32</v>
       </c>
       <c r="B23">
-        <v>125.244</v>
+        <v>125.366</v>
       </c>
       <c r="C23">
-        <v>184.50299999999999</v>
+        <v>185.36</v>
       </c>
       <c r="D23">
         <v>192.20400000000001</v>
       </c>
       <c r="E23">
-        <v>170.16800000000001</v>
+        <v>185.57499999999999</v>
       </c>
       <c r="F23">
         <v>170.02</v>
       </c>
       <c r="G23">
-        <f>2*G22</f>
+        <f t="shared" si="12"/>
         <v>195.94784000000001</v>
       </c>
       <c r="H23">
-        <f t="shared" si="10"/>
-        <v>0.63917009751166431</v>
+        <f t="shared" si="13"/>
+        <v>0.63979271218299727</v>
       </c>
       <c r="I23">
-        <f t="shared" si="11"/>
-        <v>0.94159241561427764</v>
+        <f t="shared" si="14"/>
+        <v>0.94596602851044442</v>
       </c>
       <c r="J23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.98089369089243339</v>
       </c>
       <c r="K23">
-        <f t="shared" si="13"/>
-        <v>0.86843519173265704</v>
+        <f t="shared" si="16"/>
+        <v>0.94706325928369495</v>
       </c>
       <c r="L23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.8676798886887449</v>
       </c>
     </row>
@@ -4838,39 +4837,39 @@
         <v>253.244</v>
       </c>
       <c r="C24">
-        <v>365.94200000000001</v>
+        <v>368.91800000000001</v>
       </c>
       <c r="D24">
         <v>381.137</v>
       </c>
       <c r="E24">
-        <v>365.15899999999999</v>
+        <v>369.42399999999998</v>
       </c>
       <c r="F24">
         <v>352.72</v>
       </c>
       <c r="G24">
-        <f>2*G23</f>
+        <f t="shared" si="12"/>
         <v>391.89568000000003</v>
       </c>
       <c r="H24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.64620258125835928</v>
       </c>
       <c r="I24">
-        <f t="shared" si="11"/>
-        <v>0.93377400842999847</v>
+        <f t="shared" si="14"/>
+        <v>0.94136786606068223</v>
       </c>
       <c r="J24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.97254708191731021</v>
       </c>
       <c r="K24">
-        <f t="shared" si="13"/>
-        <v>0.93177602774289314</v>
+        <f t="shared" si="16"/>
+        <v>0.9426590259938562</v>
       </c>
       <c r="L24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.90003543800227648</v>
       </c>
     </row>
@@ -4885,7 +4884,7 @@
         <v>728.92899999999997</v>
       </c>
       <c r="D25">
-        <v>746.83799999999997</v>
+        <v>763.86599999999999</v>
       </c>
       <c r="E25">
         <v>747.11699999999996</v>
@@ -4894,27 +4893,27 @@
         <v>679.76900000000001</v>
       </c>
       <c r="G25">
-        <f>2*G24</f>
+        <f t="shared" si="12"/>
         <v>783.79136000000005</v>
       </c>
       <c r="H25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.63070611036079804</v>
       </c>
       <c r="I25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.93000387245911964</v>
       </c>
       <c r="J25">
-        <f t="shared" si="12"/>
-        <v>0.95285306538719683</v>
+        <f t="shared" si="15"/>
+        <v>0.97457823469756022</v>
       </c>
       <c r="K25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.95320902746363512</v>
       </c>
       <c r="L25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.86728309942074377</v>
       </c>
     </row>
@@ -4938,27 +4937,27 @@
         <v>1345.62</v>
       </c>
       <c r="G26">
-        <f>2*G25</f>
+        <f t="shared" si="12"/>
         <v>1567.5827200000001</v>
       </c>
       <c r="H26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.63630134937950833</v>
       </c>
       <c r="I26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.93151065099773489</v>
       </c>
       <c r="J26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.96371309834290586</v>
       </c>
       <c r="K26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.86571508009478426</v>
       </c>
       <c r="L26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.85840446110556756</v>
       </c>
     </row>
@@ -4982,27 +4981,27 @@
         <v>2674.53</v>
       </c>
       <c r="G27">
-        <f>2*G26</f>
+        <f t="shared" si="12"/>
         <v>3135.1654400000002</v>
       </c>
       <c r="H27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.63404947459487171</v>
       </c>
       <c r="I27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.90757570994403403</v>
       </c>
       <c r="J27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.93854696229363888</v>
       </c>
       <c r="K27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.89992380115034687</v>
       </c>
       <c r="L27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.85307459883201575</v>
       </c>
     </row>
@@ -5026,27 +5025,27 @@
         <v>5271.18</v>
       </c>
       <c r="G28">
-        <f>2*G27</f>
+        <f t="shared" si="12"/>
         <v>6270.3308800000004</v>
       </c>
       <c r="H28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.6283352625882479</v>
       </c>
       <c r="I28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.88555135387049932</v>
       </c>
       <c r="J28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.92762249892624482</v>
       </c>
       <c r="K28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.8540426498194621</v>
       </c>
       <c r="L28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.84065420164876525</v>
       </c>
     </row>

</xml_diff>